<commit_message>
Updating with proper kelp info and additional kelp data cleaning.
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/SW Shoals Entry 2014/SW Shoals 2014 Kelp Entry.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/SW Shoals Entry 2014/SW Shoals 2014 Kelp Entry.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25040" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="36">
   <si>
     <t>YEAR</t>
   </si>
@@ -129,9 +129,6 @@
     </r>
   </si>
   <si>
-    <t>SW Appledore</t>
-  </si>
-  <si>
     <t>Katy &amp; Alison</t>
   </si>
   <si>
@@ -139,12 +136,6 @@
   </si>
   <si>
     <t>AGCL</t>
-  </si>
-  <si>
-    <t>North Smith Cove</t>
-  </si>
-  <si>
-    <t>South Smith Cove</t>
   </si>
   <si>
     <t>"ripped at tip?"</t>
@@ -156,21 +147,38 @@
   <si>
     <t>*all Ssmith entered SP on sheet</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOUTH_PEPPERRELL</t>
+  </si>
+  <si>
+    <t>NORTH_PEPPERRELL</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>KDB</t>
+  </si>
+  <si>
+    <t>SW_APPLEDORE</t>
+  </si>
+  <si>
+    <t>NORTH_SMITHS_COVE</t>
+  </si>
+  <si>
+    <t>SOUTH_SMITHS_COVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,18 +249,12 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,8 +266,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -312,13 +322,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -643,20 +661,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:O22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -725,10 +744,10 @@
         <v>41837</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -743,10 +762,13 @@
         <v>52</v>
       </c>
       <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
-        <v>25</v>
+      <c r="O2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -763,10 +785,10 @@
         <v>41837</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -781,10 +803,13 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
-        <v>25</v>
+      <c r="O3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -801,10 +826,10 @@
         <v>41837</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -819,10 +844,13 @@
         <v>39</v>
       </c>
       <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="N4" t="s">
-        <v>25</v>
+      <c r="O4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -839,10 +867,10 @@
         <v>41837</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -857,10 +885,13 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="N5" t="s">
-        <v>25</v>
+      <c r="O5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -877,10 +908,10 @@
         <v>41837</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -895,10 +926,13 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="s">
-        <v>25</v>
+      <c r="O6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -915,10 +949,10 @@
         <v>41837</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
@@ -933,10 +967,13 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="N7" t="s">
-        <v>25</v>
+      <c r="O7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -953,10 +990,10 @@
         <v>41837</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
@@ -971,10 +1008,13 @@
         <v>4</v>
       </c>
       <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="N8" t="s">
-        <v>25</v>
+      <c r="O8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -991,10 +1031,10 @@
         <v>41837</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
@@ -1009,10 +1049,13 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="N9" t="s">
-        <v>25</v>
+      <c r="O9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1029,10 +1072,10 @@
         <v>41837</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -1047,10 +1090,13 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="N10" t="s">
-        <v>25</v>
+      <c r="O10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1067,10 +1113,10 @@
         <v>41837</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
         <v>21</v>
@@ -1085,10 +1131,13 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
         <v>24</v>
       </c>
-      <c r="N11" t="s">
-        <v>25</v>
+      <c r="O11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1105,10 +1154,10 @@
         <v>41837</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
       </c>
       <c r="G12" t="s">
         <v>21</v>
@@ -1123,10 +1172,13 @@
         <v>2</v>
       </c>
       <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
         <v>24</v>
       </c>
-      <c r="N12" t="s">
-        <v>25</v>
+      <c r="O12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1143,13 +1195,13 @@
         <v>41837</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13">
         <v>55</v>
@@ -1161,10 +1213,13 @@
         <v>4</v>
       </c>
       <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="N13" t="s">
-        <v>25</v>
+      <c r="O13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1181,10 +1236,10 @@
         <v>41837</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>21</v>
@@ -1199,13 +1254,16 @@
         <v>2</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N14" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1222,10 +1280,10 @@
         <v>41837</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>21</v>
@@ -1234,16 +1292,19 @@
         <v>59.5</v>
       </c>
       <c r="I15" s="1">
-        <v>1.6</v>
+        <v>16</v>
       </c>
       <c r="J15">
         <v>2.8</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="O15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1260,10 +1321,10 @@
         <v>41837</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>21</v>
@@ -1278,13 +1339,16 @@
         <v>3</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="O16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -1298,10 +1362,10 @@
         <v>41837</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>21</v>
@@ -1316,13 +1380,16 @@
         <v>5.5</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="O17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>2014</v>
       </c>
@@ -1336,10 +1403,10 @@
         <v>41837</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>21</v>
@@ -1354,13 +1421,16 @@
         <v>2.5</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="O18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>2014</v>
       </c>
@@ -1374,10 +1444,10 @@
         <v>41837</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>21</v>
@@ -1392,16 +1462,19 @@
         <v>4.5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="O19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>2014</v>
       </c>
@@ -1415,10 +1488,10 @@
         <v>41837</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>21</v>
@@ -1433,13 +1506,16 @@
         <v>0.6</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="O20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -1453,10 +1529,10 @@
         <v>41837</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>21</v>
@@ -1471,17 +1547,1205 @@
         <v>1.4</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>183</v>
+      </c>
+      <c r="I22">
+        <v>23</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23">
+        <v>41</v>
+      </c>
+      <c r="I23">
+        <v>13</v>
+      </c>
+      <c r="J23">
+        <v>1.5</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N23" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>2014</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>19</v>
+      </c>
+      <c r="D24" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>1.5</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25">
+        <v>28.5</v>
+      </c>
+      <c r="I25">
+        <v>7</v>
+      </c>
+      <c r="J25">
+        <v>2.5</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>19</v>
+      </c>
+      <c r="D26" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26">
+        <v>40.5</v>
+      </c>
+      <c r="I26">
+        <v>20</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N26" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="D27" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27">
+        <v>44</v>
+      </c>
+      <c r="I27">
+        <v>16</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N27" t="s">
+        <v>31</v>
+      </c>
+      <c r="O27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>2014</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <v>49</v>
+      </c>
+      <c r="I28">
+        <v>13</v>
+      </c>
+      <c r="J28">
+        <v>2.5</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" t="s">
+        <v>31</v>
+      </c>
+      <c r="O28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="D29" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29">
+        <v>20</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>19</v>
+      </c>
+      <c r="D30" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>16</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" t="s">
+        <v>31</v>
+      </c>
+      <c r="O30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+      <c r="D31" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31">
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N31" t="s">
+        <v>31</v>
+      </c>
+      <c r="O31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>19</v>
+      </c>
+      <c r="D32" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32">
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <v>7.5</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="D33" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33">
+        <v>24</v>
+      </c>
+      <c r="I33">
+        <v>11.5</v>
+      </c>
+      <c r="J33">
+        <v>4.5</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N33" t="s">
+        <v>31</v>
+      </c>
+      <c r="O33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>19</v>
+      </c>
+      <c r="D34" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N21" t="s">
+      <c r="G34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34">
+        <v>357</v>
+      </c>
+      <c r="I34">
+        <v>45</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" t="s">
+        <v>31</v>
+      </c>
+      <c r="O34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>19</v>
+      </c>
+      <c r="D35" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35">
+        <v>220</v>
+      </c>
+      <c r="I35">
+        <v>47</v>
+      </c>
+      <c r="J35">
+        <v>4.5</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36">
+        <v>60</v>
+      </c>
+      <c r="I36">
+        <v>15</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" t="s">
+        <v>31</v>
+      </c>
+      <c r="O36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>19</v>
+      </c>
+      <c r="D37" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37">
+        <v>85</v>
+      </c>
+      <c r="I37">
+        <v>18</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37" t="s">
+        <v>31</v>
+      </c>
+      <c r="O37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>19</v>
+      </c>
+      <c r="D38" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38">
+        <v>56</v>
+      </c>
+      <c r="I38">
+        <v>15</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" t="s">
+        <v>31</v>
+      </c>
+      <c r="O38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>19</v>
+      </c>
+      <c r="D39" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39">
+        <v>19</v>
+      </c>
+      <c r="I39">
+        <v>5.5</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" t="s">
+        <v>31</v>
+      </c>
+      <c r="O39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="D40" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40">
+        <v>31.5</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>1.5</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" t="s">
+        <v>31</v>
+      </c>
+      <c r="O40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41">
+        <v>2014</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>19</v>
+      </c>
+      <c r="D41" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41">
+        <v>17.5</v>
+      </c>
+      <c r="I41">
+        <v>6.5</v>
+      </c>
+      <c r="J41">
+        <v>0.5</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" t="s">
+        <v>31</v>
+      </c>
+      <c r="O41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42">
+        <v>2014</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+      <c r="D42" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42">
+        <v>54</v>
+      </c>
+      <c r="I42">
+        <v>13</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" t="s">
+        <v>31</v>
+      </c>
+      <c r="O42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43">
+        <v>2014</v>
+      </c>
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>19</v>
+      </c>
+      <c r="D43" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43">
+        <v>23.5</v>
+      </c>
+      <c r="I43">
+        <v>7</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" t="s">
+        <v>31</v>
+      </c>
+      <c r="O43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>19</v>
+      </c>
+      <c r="D44" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44">
+        <v>48.5</v>
+      </c>
+      <c r="I44">
+        <v>15</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45">
+        <v>2014</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>19</v>
+      </c>
+      <c r="D45" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45">
+        <v>28</v>
+      </c>
+      <c r="I45">
+        <v>7</v>
+      </c>
+      <c r="J45">
+        <v>1.5</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" t="s">
+        <v>31</v>
+      </c>
+      <c r="O45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46">
+        <v>2014</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>19</v>
+      </c>
+      <c r="D46" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46">
+        <v>33.5</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>1.5</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" t="s">
+        <v>31</v>
+      </c>
+      <c r="O46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47">
+        <v>2014</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>19</v>
+      </c>
+      <c r="D47" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47">
+        <v>44</v>
+      </c>
+      <c r="I47">
+        <v>8.5</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" t="s">
+        <v>31</v>
+      </c>
+      <c r="O47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48">
+        <v>2014</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>19</v>
+      </c>
+      <c r="D48" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48">
+        <v>34</v>
+      </c>
+      <c r="I48">
+        <v>9.5</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N48" t="s">
+        <v>31</v>
+      </c>
+      <c r="O48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>2014</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>19</v>
+      </c>
+      <c r="D49" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49">
+        <v>37.5</v>
+      </c>
+      <c r="I49">
+        <v>17</v>
+      </c>
+      <c r="J49">
+        <v>1.5</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N49" t="s">
+        <v>31</v>
+      </c>
+      <c r="O49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <v>2014</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>19</v>
+      </c>
+      <c r="D50" s="10">
+        <v>41839</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="L22" s="1"/>
+      <c r="H50">
+        <v>30.5</v>
+      </c>
+      <c r="I50">
+        <v>35.5</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N50" t="s">
+        <v>31</v>
+      </c>
+      <c r="O50" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1496,7 +2760,7 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1504,14 +2768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11"/>
@@ -1562,11 +2826,10 @@
       <c r="D5" s="14"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>